<commit_message>
added more menus and a news post
</commit_message>
<xml_diff>
--- a/_content/allmenu.xlsx
+++ b/_content/allmenu.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17301"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chryw\Dropbox\Work\githubrepo\hoh\_content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-cherrw\Dropbox\Work\githubrepo\hoh\_content\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9720"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="fullmenu" sheetId="1" r:id="rId1"/>
+    <sheet name="setmenu" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="272">
   <si>
     <t>Fried pork intestines</t>
   </si>
@@ -549,6 +550,381 @@
   </si>
   <si>
     <t>熏魚</t>
+  </si>
+  <si>
+    <t>經典家庭套餐</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Classical Mandarin Family Dinner Set </t>
+  </si>
+  <si>
+    <t xml:space="preserve">北京烤鴨 </t>
+  </si>
+  <si>
+    <t>海鮮魚肚羹</t>
+  </si>
+  <si>
+    <t>Seafood fish maw soup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">核桃蝦球 </t>
+  </si>
+  <si>
+    <t>Walnut prawns salad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">時菜斑球 </t>
+  </si>
+  <si>
+    <t>Cod filet with vegetables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">貴妃走地鷄 </t>
+  </si>
+  <si>
+    <t>Range free chicken</t>
+  </si>
+  <si>
+    <t xml:space="preserve">金菇扒玉蘭 </t>
+  </si>
+  <si>
+    <r>
+      <t>蒙古牛肉</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">椒鹽肉排 </t>
+  </si>
+  <si>
+    <t>Pepper salt pork chops</t>
+  </si>
+  <si>
+    <t xml:space="preserve">海鮮蘭粒炒飯 </t>
+  </si>
+  <si>
+    <t>Seafood broccoli fried rice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">甜品或生果 </t>
+  </si>
+  <si>
+    <t>Dessert or seasonal fruit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">豪華家庭套餐 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">House of Hong Mandarin Family Dinner Set </t>
+  </si>
+  <si>
+    <t xml:space="preserve">蟹肉魚肚羹 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">新疆羊肉 </t>
+  </si>
+  <si>
+    <r>
+      <t>辣子龍蝦蟹</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Five-star spicy lobster and crab</t>
+  </si>
+  <si>
+    <r>
+      <t>貴妃走地鷄</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>素黃雀</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">豆瓣全魚 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">京都肉排 </t>
+  </si>
+  <si>
+    <t>Royal Peking pork chops</t>
+  </si>
+  <si>
+    <r>
+      <t>福州炒飯</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Fuzhou fried rice</t>
+  </si>
+  <si>
+    <r>
+      <t>甜品或生果</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">精品個人套餐 </t>
+  </si>
+  <si>
+    <t>Individual Mandarin Dinner Set</t>
+  </si>
+  <si>
+    <t>Egg Roll</t>
+  </si>
+  <si>
+    <t>Deep fried prawns</t>
+  </si>
+  <si>
+    <t>Wonton soup</t>
+  </si>
+  <si>
+    <t>Chicken with mixed vegetables</t>
+  </si>
+  <si>
+    <t>(3 persons add Moo-shu pork)</t>
+  </si>
+  <si>
+    <t>(4 persons add Walnut prawn salad)</t>
+  </si>
+  <si>
+    <t>炸蝦</t>
+  </si>
+  <si>
+    <t>叉燒</t>
+  </si>
+  <si>
+    <t>雲吞麵</t>
+  </si>
+  <si>
+    <t>蒙古牛</t>
+  </si>
+  <si>
+    <t>三人以上加木須肉</t>
+  </si>
+  <si>
+    <t>四人以上加核桃蝦</t>
+  </si>
+  <si>
+    <r>
+      <t>川菜個人套餐</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Individual Szechuan Dinner Set</t>
+  </si>
+  <si>
+    <t>Spicy basil beef with mixed vegetables</t>
+  </si>
+  <si>
+    <t>General Tsao’s chicken</t>
+  </si>
+  <si>
+    <t>麻辣牛肉小炒</t>
+  </si>
+  <si>
+    <t>左宗棠雞</t>
+  </si>
+  <si>
+    <t>evening_dimsum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">炸春卷 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">鍋貼 </t>
+  </si>
+  <si>
+    <t>鳳爪</t>
+  </si>
+  <si>
+    <t>豆豉蒸排骨</t>
+  </si>
+  <si>
+    <t>Spareribs in black bean sauce</t>
+  </si>
+  <si>
+    <t>鮮竹卷</t>
+  </si>
+  <si>
+    <t xml:space="preserve">燒賣 </t>
+  </si>
+  <si>
+    <t>帶子餃</t>
+  </si>
+  <si>
+    <t>香茜較</t>
+  </si>
+  <si>
+    <t>蝦餃</t>
+  </si>
+  <si>
+    <t>蒸叉烧包</t>
+  </si>
+  <si>
+    <t>Pork Egg Rolls</t>
+  </si>
+  <si>
+    <t>Pork egg rolls</t>
+  </si>
+  <si>
+    <t>Pan-seared pork potstickers</t>
+  </si>
+  <si>
+    <t>Steamed chicken feet</t>
+  </si>
+  <si>
+    <t>Pork bean curd rolls</t>
+  </si>
+  <si>
+    <t>Pork siu mai dumplings</t>
+  </si>
+  <si>
+    <t>Scallop &amp; shrimp dumplings</t>
+  </si>
+  <si>
+    <t>Shrimp &amp; cilantro dumplings</t>
+  </si>
+  <si>
+    <t>Shrimp har gow dumplings</t>
+  </si>
+  <si>
+    <t>Steamed barbeque pork buns</t>
+  </si>
+  <si>
+    <t>dimsum</t>
+  </si>
+  <si>
+    <t>lunch special</t>
+  </si>
+  <si>
+    <t>lunch</t>
+  </si>
+  <si>
+    <t>甜酸雞</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweet &amp; sour chicken </t>
+  </si>
+  <si>
+    <t xml:space="preserve">杏仁雞 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Almond chicken </t>
+  </si>
+  <si>
+    <t xml:space="preserve">時菜雞 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chicken with mixed vegetables </t>
+  </si>
+  <si>
+    <t xml:space="preserve">時菜豆腐 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tofu with mixed vegetables </t>
+  </si>
+  <si>
+    <t xml:space="preserve">蒙古牛肉 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mongolian beef </t>
+  </si>
+  <si>
+    <t xml:space="preserve">西蘭花牛肉 </t>
+  </si>
+  <si>
+    <t>甜酸肉</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweet &amp; sour pork </t>
+  </si>
+  <si>
+    <t xml:space="preserve">宮保蝦球 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kung Pao prawns </t>
+  </si>
+  <si>
+    <t xml:space="preserve">時菜蝦球 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prawns with mixed vegetables </t>
+  </si>
+  <si>
+    <t xml:space="preserve">乾炒牛河 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dry beef chow fon </t>
   </si>
 </sst>
 </file>
@@ -584,8 +960,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -902,17 +1285,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="58.19921875" customWidth="1"/>
-    <col min="7" max="7" width="13.86328125" customWidth="1"/>
+    <col min="2" max="3" width="58.25" customWidth="1"/>
+    <col min="7" max="7" width="13.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>171</v>
       </c>
@@ -932,7 +1315,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -957,7 +1340,7 @@
         <v>- id: 1%name_en: "Fried vegetable spring rolls"%name_ch: "炸春卷"%price: 3.95%type: "appetizer"</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -982,7 +1365,7 @@
         <v>- id: 2%name_en: "Pot stickers (or steamed)"%name_ch: "煎鍋貼 (或蒸餃)"%price: 7.95%type: "appetizer"</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1007,7 +1390,7 @@
         <v>- id: 3%name_en: "Barbecued pork"%name_ch: "叉烧"%price: 7.95%type: "appetizer"</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1032,7 +1415,7 @@
         <v>- id: 4%name_en: "Green onion pancakes"%name_ch: "葱油餅"%price: 4.95%type: "appetizer"</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1057,7 +1440,7 @@
         <v>- id: 5%name_en: "Fried garlic chicken wings"%name_ch: "炸蒜香鷄翼"%price: 6.95%type: "appetizer"</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1082,7 +1465,7 @@
         <v>- id: 6%name_en: " Cold jellyfish salad"%name_ch: "涼拌海蜇"%price: 8.95%type: "appetizer"</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1110,7 +1493,7 @@
         <v>- id: 7%name_en: "Beef tendon with hot sauce"%name_ch: "麻辣牛筋"%price: 7.95%spicy: 2%type: "appetizer"</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1138,7 +1521,7 @@
         <v>- id: 8%name_en: "Shredded beef tripe with hot sauce"%name_ch: "紅油肚絲"%price: 7.95%spicy: 2%type: "appetizer"</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1166,7 +1549,7 @@
         <v>- id: 9%name_en: "Cold spicy smoked fish"%name_ch: "熏魚"%price: 7.95%spicy: 2%type: "appetizer"</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1191,7 +1574,7 @@
         <v>- id: 10%name_en: "Fried pork intestines"%name_ch: "炸大腸"%price: 7.95%type: "appetizer"</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1216,7 +1599,7 @@
         <v>- id: 11%name_en: "Steamed mini pork buns"%name_ch: "小籠包"%price: 7.95%type: "carbappetizer"</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1241,7 +1624,7 @@
         <v>- id: 12%name_en: "Noodles in Szechuan hot sauce"%name_ch: "擔擔麵"%price: 5.95%type: "carbappetizer"</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1266,7 +1649,7 @@
         <v>- id: 13%name_en: "Chilled noodles in Szechuan sesame sauce"%name_ch: "涼麵"%price: 5.95%type: "carbappetizer"</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1291,7 +1674,7 @@
         <v>- id: 14%name_en: "Homemade pan fried noodles Shanghai style"%name_ch: "上海炒粗麵"%price: 7.95%type: "carbappetizer"</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1319,7 +1702,7 @@
         <v>- id: 15%name_en: "Hot &amp; sour soup"%name_ch: "酸辣湯"%price: 7.5%spicy: 1%type: "soup"</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1344,7 +1727,7 @@
         <v>- id: 16%name_en: "Egg flower soup"%name_ch: "蛋花湯"%price: 7.5%type: "soup"</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1369,7 +1752,7 @@
         <v>- id: 17%name_en: "BBQ pork wonton soup"%name_ch: "雲吞湯"%price: 7.25%type: "soup"</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1394,7 +1777,7 @@
         <v>- id: 18%name_en: "Sizzling rice cake &amp; seafood soup"%name_ch: "海鮮鍋巴湯"%price: 10.25%type: "soup"</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1419,7 +1802,7 @@
         <v>- id: 19%name_en: "Seafood tofu soup"%name_ch: "海鮮豆腐羹"%price: 10.25%type: "soup"</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1444,7 +1827,7 @@
         <v>- id: 20%name_en: "Fish maw with crab meat soup"%name_ch: "蟹肉魚肚羹"%price: 13.95%type: "soup"</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1472,7 +1855,7 @@
         <v>- id: 21%name_en: "Five-star spicy crispy scallops with garlic and chili pepper"%name_ch: "香辣乾貝"%price: 18.5%spicy: 3%type: "szechuan"</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1497,7 +1880,7 @@
         <v>- id: 22%name_en: "Five-star spicy crab with chili peppers"%name_ch: "香辣蟹"%price: %spicy: 3%type: "szechuan"</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1525,7 +1908,7 @@
         <v>- id: 23%name_en: "Spicy prawn on soybean cake"%name_ch: "豆花蝦"%price: 17.5%spicy: 3%type: "szechuan"</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1553,7 +1936,7 @@
         <v>- id: 24%name_en: "Spicy pan fried noodles with choice of chicken, beef, pork, or prawn"%name_ch: "香辣炒面"%price: 10.5%spicy: 3%type: "szechuan"</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1581,7 +1964,7 @@
         <v>- id: 25%name_en: "Five-star spicy chicken with chili peppers"%name_ch: "辣子鷄"%price: 11.95%spicy: 3%type: "szechuan"</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1609,7 +1992,7 @@
         <v>- id: 26%name_en: "Poached sliced beef in chili oil"%name_ch: "水煮牛肉"%price: 12.95%spicy: 3%type: "szechuan"</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1637,7 +2020,7 @@
         <v>- id: 27%name_en: "Poached fish fillet in hot chili oil"%name_ch: "水煮魚"%price: 12.95%spicy: 3%type: "szechuan"</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1665,7 +2048,7 @@
         <v>- id: 28%name_en: "Fish fillet with pickled chili peppers"%name_ch: "泡椒魚"%price: 16.95%spicy: 3%type: "szechuan"</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1693,7 +2076,7 @@
         <v>- id: 29%name_en: "Spicy fish fillet on soybean cake"%name_ch: "豆花魚"%price: 17.95%spicy: 3%type: "szechuan"</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1721,7 +2104,7 @@
         <v>- id: 30%name_en: "Sautéed lamb with triple chili peppers"%name_ch: "三椒羊肉"%price: 17.95%spicy: 3%type: "szechuan"</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1749,7 +2132,7 @@
         <v>- id: 31%name_en: "Spicy lamb with cumin flavor"%name_ch: "新疆羊肉"%price: 18.95%spicy: 3%type: "szechuan"</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1777,7 +2160,7 @@
         <v>- id: 32%name_en: "General Chiang’s beef brisket"%name_ch: "張飛牛腩 "%price: 14.95%spicy: 3%type: "szechuan"</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1805,7 +2188,7 @@
         <v>- id: 33%name_en: "Crispy pork intestines with garlic and chili peppers"%name_ch: "山椒脆腸"%price: 12.95%spicy: 3%type: "szechuan"</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1830,7 +2213,7 @@
         <v>- id: 34%name_en: "Fried tofu"%name_ch: "炸豆腐"%price: 7.5%type: "vegetable"</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1855,7 +2238,7 @@
         <v>- id: 35%name_en: "Bean curd wrapped enoki and shiitake mushrooms"%name_ch: "素黃雀"%price: 11.95%type: "vegetable"</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1880,7 +2263,7 @@
         <v>- id: 36%name_en: "Enoki &amp; shiitake mushrooms with Chinese broccoli"%name_ch: "金菇扒玉蘭"%price: 11.95%type: "vegetable"</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1905,7 +2288,7 @@
         <v>- id: 37%name_en: "Mandarin style mixed vegetables"%name_ch: "素什錦"%price: 9.95%type: "vegetable"</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1930,7 +2313,7 @@
         <v>- id: 38%name_en: "Chinese broccoli with oyster sauce"%name_ch: "蠔油芥藍"%price: 9.95%type: "vegetable"</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1955,7 +2338,7 @@
         <v>- id: 39%name_en: "Oyster mushrooms with seasonal vegetables"%name_ch: "靈芝菇扒時蔬"%price: 12.95%type: "vegetable"</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1980,7 +2363,7 @@
         <v>- id: 40%name_en: "Pea vines in garlic sauce"%name_ch: "蒜蓉炒豆苗"%price: 16.95%type: "vegetable"</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2005,7 +2388,7 @@
         <v>- id: 41%name_en: "Shiitake &amp; Snow peas with broccoli in oyster sauce"%name_ch: "素三鮮"%price: 10.95%type: "vegetable"</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2030,7 +2413,7 @@
         <v>- id: 42%name_en: "Eggplant in Szechuan garlic sauce"%name_ch: "魚香茄子"%price: 10.95%type: "vegetable"</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2058,7 +2441,7 @@
         <v>- id: 43%name_en: "Vegetarian dry sautéed string beans"%name_ch: "乾煸四季豆"%price: 10.95%spicy: 2%type: "vegetable"</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2083,7 +2466,7 @@
         <v>- id: 44%name_en: "Sautéed string beans"%name_ch: "炒四季豆"%price: 10.5%type: "vegetable"</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2108,7 +2491,7 @@
         <v>- id: 45%name_en: "Egg Foo Young with choice of BBQ pork, chicken or beef"%name_ch: "各式芙蓉蛋炒肉"%price: 9.95%type: "eggfooyoung"</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2133,7 +2516,7 @@
         <v>- id: 46%name_en: "Vegetable Egg Foo Young"%name_ch: "素芙蓉蛋 "%price: 8.95%type: "eggfooyoung"</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2158,7 +2541,7 @@
         <v>- id: 47%name_en: "Prawn Egg Foo Young"%name_ch: "芙蓉蛋炒蝦"%price: 11.95%type: "eggfooyoung"</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2186,7 +2569,7 @@
         <v>- id: 48%name_en: "Prawn with peanuts in hot pepper sauce"%name_ch: "宮保蝦球"%price: 15.95%spicy: 2%type: "seafood"</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2214,7 +2597,7 @@
         <v>- id: 49%name_en: "Prawn with pepper sauce"%name_ch: "鹽酥蝦 "%price: 17.95%spicy: 2%type: "seafood"</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2239,7 +2622,7 @@
         <v>- id: 50%name_en: "Walnut prawn salad"%name_ch: "核桃蝦"%price: 18.95%type: "seafood"</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2264,7 +2647,7 @@
         <v>- id: 51%name_en: "Prawn with snow peas"%name_ch: "雪豆蝦球"%price: 17.95%type: "seafood"</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2289,7 +2672,7 @@
         <v>- id: 52%name_en: "Sweet &amp; sour prawn"%name_ch: "甜酸蝦球 "%price: 14.95%type: "seafood"</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2317,7 +2700,7 @@
         <v>- id: 53%name_en: "Whole fish with spicy black bean sauce"%name_ch: "豆瓣全魚"%price: 15.95%spicy: 2%type: "seafood"</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2345,7 +2728,7 @@
         <v>- id: 54%name_en: "Spicy basil prawn with vegetables"%name_ch: "九層塔蝦"%price: 17.5%spicy: 2%type: "seafood"</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2370,7 +2753,7 @@
         <v>- id: 55%name_en: "Sliced pork with preserved vegetables"%name_ch: "蒜泥白肉"%price: 12.95%type: "meat"</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2395,7 +2778,7 @@
         <v>- id: 56%name_en: "Sliced pork with cabbage"%name_ch: "回鍋肉"%price: 12.95%type: "meat"</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2420,7 +2803,7 @@
         <v>- id: 57%name_en: "Shredded pork with dried bean curd &amp; yellow leeks"%name_ch: "韭黃香乾肉絲"%price: 13.95%type: "meat"</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2445,7 +2828,7 @@
         <v>- id: 58%name_en: "Shredded pork &amp; squid with dried bean curd &amp; yellow leeks"%name_ch: "韭黃香乾魷魚絲"%price: 15.95%type: "meat"</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2470,7 +2853,7 @@
         <v>- id: 59%name_en: "Curry chicken"%name_ch: "咖喱鷄"%price: 11.95%type: "meat"</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2495,7 +2878,7 @@
         <v>- id: 60%name_en: "Spicy basil chicken casserole"%name_ch: "三杯鷄"%price: 12.95%type: "meat"</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2520,7 +2903,7 @@
         <v>- id: 61%name_en: "Crispy chicken with salt &amp; pepper"%name_ch: "鹽酥鷄"%price: 12.95%type: "meat"</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2545,7 +2928,7 @@
         <v>- id: 62%name_en: "Almond fried chicken"%name_ch: "杏仁雞"%price: 10.5%type: "meat"</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2570,7 +2953,7 @@
         <v>- id: 63%name_en: "Range free chicken (half)"%name_ch: "貴妃雞"%price: 10.5%type: "meat"</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2595,7 +2978,7 @@
         <v>- id: 64%name_en: "Roasted duck (half)"%name_ch: "燒鴨"%price: 10.5%type: "meat"</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2620,7 +3003,7 @@
         <v>- id: 65%name_en: "Royal Peking duck"%name_ch: "北京烤鴨"%price: 32%type: "meat"</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2645,7 +3028,7 @@
         <v>- id: 66%name_en: "Beef tripe sautéed with bean sprouts"%name_ch: "銀芽毛肚"%price: 12.95%type: "meat"</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -2670,7 +3053,7 @@
         <v>- id: 67%name_en: "Tea smoked duck (half) "%name_ch: "樟茶鴨"%price: 14.25%type: "meat"</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -2698,7 +3081,7 @@
         <v>- id: 68%name_en: "Spicy pork intestines with pickled vegetables hot pot"%name_ch: "五更腸旺"%price: 12.95%spicy: 2%type: "meat"</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -2723,7 +3106,7 @@
         <v>- id: 69%name_en: "Mongolian beef"%name_ch: "蒙古牛肉"%price: 14.95%type: "meat"</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -2748,7 +3131,7 @@
         <v>- id: 70%name_en: "Beef with broccoli"%name_ch: "西蘭花牛肉"%price: 14.5%type: "meat"</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -2773,7 +3156,7 @@
         <v>- id: 71%name_en: "Fried rice with choice of BBQ pork, chicken, beef or prawn"%name_ch: "各式炒飯 "%price: 8.5%type: "carb"</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -2798,7 +3181,7 @@
         <v>- id: 72%name_en: "Dried beef chow fon"%name_ch: "乾炒牛河"%price: 10.75%type: "carb"</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -2826,7 +3209,7 @@
         <v>- id: 73%name_en: "Singapore style vermicelli "%name_ch: "星洲炒米粉"%price: 9.25%spicy: 2%type: "carb"</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -2851,7 +3234,7 @@
         <v>- id: 74%name_en: "Seafood chow mein"%name_ch: "海鮮炒麵"%price: 10.95%type: "carb"</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -2876,7 +3259,7 @@
         <v>- id: 75%name_en: "Vegetable chow mein"%name_ch: "素菜炒麵"%price: 8.5%type: "carb"</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -2901,7 +3284,7 @@
         <v>- id: 76%name_en: "House special chow mein "%name_ch: "招牌炒麵"%price: 10.75%type: "carb"</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -2926,7 +3309,7 @@
         <v>- id: 77%name_en: "Pan fried noodle with choice of BBQ pork, chicken, beef or prawn"%name_ch: "各式炒麵"%price: 8.95%type: "carb"</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -2951,7 +3334,7 @@
         <v>- id: 78%name_en: "Wonton noodle soup"%name_ch: "雲吞湯麵"%price: 7.5%type: "carb"</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -2976,7 +3359,7 @@
         <v>- id: 79%name_en: "Roasted duck noodle soup"%name_ch: "燒鴨湯麵"%price: 7.5%type: "carb"</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -3005,4 +3388,928 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I69"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="I58" sqref="I58:I69"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="25.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D2" s="1">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B38" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B39" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B42" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B43" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B45" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C45" s="1"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>1</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F46">
+        <v>4.5</v>
+      </c>
+      <c r="G46" t="s">
+        <v>250</v>
+      </c>
+      <c r="H46" t="str">
+        <f>_xlfn.CONCAT("- id: ",A46,"%name_en: '",C46,"'%name_ch: '",B46,"'%price: ",F46,IF(LEN(F46)&gt;0,(_xlfn.CONCAT("%spicy: ",E46)),""),"%type: '",G46,"'")</f>
+        <v>- id: 1%name_en: 'Pork egg rolls'%name_ch: '炸春卷 '%price: 4.5%spicy: %type: 'dimsum'</v>
+      </c>
+      <c r="I46" t="str">
+        <f>SUBSTITUTE(H46,"'","""")</f>
+        <v>- id: 1%name_en: "Pork egg rolls"%name_ch: "炸春卷 "%price: 4.5%spicy: %type: "dimsum"</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>2</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="F47">
+        <v>4.5</v>
+      </c>
+      <c r="G47" t="s">
+        <v>250</v>
+      </c>
+      <c r="H47" t="str">
+        <f t="shared" ref="H47:H55" si="0">_xlfn.CONCAT("- id: ",A47,"%name_en: '",C47,"'%name_ch: '",B47,"'%price: ",F47,IF(LEN(F47)&gt;0,(_xlfn.CONCAT("%spicy: ",E47)),""),"%type: '",G47,"'")</f>
+        <v>- id: 2%name_en: 'Pan-seared pork potstickers'%name_ch: '鍋貼 '%price: 4.5%spicy: %type: 'dimsum'</v>
+      </c>
+      <c r="I47" t="str">
+        <f t="shared" ref="I47:I55" si="1">SUBSTITUTE(H47,"'","""")</f>
+        <v>- id: 2%name_en: "Pan-seared pork potstickers"%name_ch: "鍋貼 "%price: 4.5%spicy: %type: "dimsum"</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>3</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="F48">
+        <v>4.5</v>
+      </c>
+      <c r="G48" t="s">
+        <v>250</v>
+      </c>
+      <c r="H48" t="str">
+        <f t="shared" si="0"/>
+        <v>- id: 3%name_en: 'Steamed chicken feet'%name_ch: '鳳爪'%price: 4.5%spicy: %type: 'dimsum'</v>
+      </c>
+      <c r="I48" t="str">
+        <f t="shared" si="1"/>
+        <v>- id: 3%name_en: "Steamed chicken feet"%name_ch: "鳳爪"%price: 4.5%spicy: %type: "dimsum"</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>4</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F49">
+        <v>4.5</v>
+      </c>
+      <c r="G49" t="s">
+        <v>250</v>
+      </c>
+      <c r="H49" t="str">
+        <f t="shared" si="0"/>
+        <v>- id: 4%name_en: 'Spareribs in black bean sauce'%name_ch: '豆豉蒸排骨'%price: 4.5%spicy: %type: 'dimsum'</v>
+      </c>
+      <c r="I49" t="str">
+        <f t="shared" si="1"/>
+        <v>- id: 4%name_en: "Spareribs in black bean sauce"%name_ch: "豆豉蒸排骨"%price: 4.5%spicy: %type: "dimsum"</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>5</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="F50">
+        <v>4.5</v>
+      </c>
+      <c r="G50" t="s">
+        <v>250</v>
+      </c>
+      <c r="H50" t="str">
+        <f t="shared" si="0"/>
+        <v>- id: 5%name_en: 'Pork bean curd rolls'%name_ch: '鮮竹卷'%price: 4.5%spicy: %type: 'dimsum'</v>
+      </c>
+      <c r="I50" t="str">
+        <f t="shared" si="1"/>
+        <v>- id: 5%name_en: "Pork bean curd rolls"%name_ch: "鮮竹卷"%price: 4.5%spicy: %type: "dimsum"</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>6</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="F51">
+        <v>4.5</v>
+      </c>
+      <c r="G51" t="s">
+        <v>250</v>
+      </c>
+      <c r="H51" t="str">
+        <f t="shared" si="0"/>
+        <v>- id: 6%name_en: 'Pork siu mai dumplings'%name_ch: '燒賣 '%price: 4.5%spicy: %type: 'dimsum'</v>
+      </c>
+      <c r="I51" t="str">
+        <f t="shared" si="1"/>
+        <v>- id: 6%name_en: "Pork siu mai dumplings"%name_ch: "燒賣 "%price: 4.5%spicy: %type: "dimsum"</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>7</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F52">
+        <v>4.5</v>
+      </c>
+      <c r="G52" t="s">
+        <v>250</v>
+      </c>
+      <c r="H52" t="str">
+        <f t="shared" si="0"/>
+        <v>- id: 7%name_en: 'Scallop &amp; shrimp dumplings'%name_ch: '帶子餃'%price: 4.5%spicy: %type: 'dimsum'</v>
+      </c>
+      <c r="I52" t="str">
+        <f t="shared" si="1"/>
+        <v>- id: 7%name_en: "Scallop &amp; shrimp dumplings"%name_ch: "帶子餃"%price: 4.5%spicy: %type: "dimsum"</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>8</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="F53">
+        <v>4.5</v>
+      </c>
+      <c r="G53" t="s">
+        <v>250</v>
+      </c>
+      <c r="H53" t="str">
+        <f t="shared" si="0"/>
+        <v>- id: 8%name_en: 'Shrimp &amp; cilantro dumplings'%name_ch: '香茜較'%price: 4.5%spicy: %type: 'dimsum'</v>
+      </c>
+      <c r="I53" t="str">
+        <f t="shared" si="1"/>
+        <v>- id: 8%name_en: "Shrimp &amp; cilantro dumplings"%name_ch: "香茜較"%price: 4.5%spicy: %type: "dimsum"</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>9</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="F54">
+        <v>4.5</v>
+      </c>
+      <c r="G54" t="s">
+        <v>250</v>
+      </c>
+      <c r="H54" t="str">
+        <f t="shared" si="0"/>
+        <v>- id: 9%name_en: 'Shrimp har gow dumplings'%name_ch: '蝦餃'%price: 4.5%spicy: %type: 'dimsum'</v>
+      </c>
+      <c r="I54" t="str">
+        <f t="shared" si="1"/>
+        <v>- id: 9%name_en: "Shrimp har gow dumplings"%name_ch: "蝦餃"%price: 4.5%spicy: %type: "dimsum"</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>10</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="F55">
+        <v>4.5</v>
+      </c>
+      <c r="G55" t="s">
+        <v>250</v>
+      </c>
+      <c r="H55" t="str">
+        <f t="shared" si="0"/>
+        <v>- id: 10%name_en: 'Steamed barbeque pork buns'%name_ch: '蒸叉烧包'%price: 4.5%spicy: %type: 'dimsum'</v>
+      </c>
+      <c r="I55" t="str">
+        <f t="shared" si="1"/>
+        <v>- id: 10%name_en: "Steamed barbeque pork buns"%name_ch: "蒸叉烧包"%price: 4.5%spicy: %type: "dimsum"</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>1</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="F58">
+        <v>7.5</v>
+      </c>
+      <c r="G58" t="s">
+        <v>252</v>
+      </c>
+      <c r="H58" t="str">
+        <f t="shared" ref="H58:H69" si="2">_xlfn.CONCAT("- id: ",A58,"%name_en: '",C58,"'%name_ch: '",B58,"'%price: ",F58,IF(LEN(F58)&gt;0,(_xlfn.CONCAT("%spicy: ",E58)),""),"%type: '",G58,"'")</f>
+        <v>- id: 1%name_en: 'General Tsao’s chicken'%name_ch: '左宗棠雞'%price: 7.5%spicy: %type: 'lunch'</v>
+      </c>
+      <c r="I58" t="str">
+        <f t="shared" ref="I58:I69" si="3">SUBSTITUTE(H58,"'","""")</f>
+        <v>- id: 1%name_en: "General Tsao’s chicken"%name_ch: "左宗棠雞"%price: 7.5%spicy: %type: "lunch"</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>2</v>
+      </c>
+      <c r="B59" t="s">
+        <v>253</v>
+      </c>
+      <c r="C59" t="s">
+        <v>254</v>
+      </c>
+      <c r="F59">
+        <v>7</v>
+      </c>
+      <c r="G59" t="s">
+        <v>252</v>
+      </c>
+      <c r="H59" t="str">
+        <f t="shared" si="2"/>
+        <v>- id: 2%name_en: 'Sweet &amp; sour chicken '%name_ch: '甜酸雞'%price: 7%spicy: %type: 'lunch'</v>
+      </c>
+      <c r="I59" t="str">
+        <f t="shared" si="3"/>
+        <v>- id: 2%name_en: "Sweet &amp; sour chicken "%name_ch: "甜酸雞"%price: 7%spicy: %type: "lunch"</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>3</v>
+      </c>
+      <c r="B60" t="s">
+        <v>255</v>
+      </c>
+      <c r="C60" t="s">
+        <v>256</v>
+      </c>
+      <c r="F60">
+        <v>7</v>
+      </c>
+      <c r="G60" t="s">
+        <v>252</v>
+      </c>
+      <c r="H60" t="str">
+        <f t="shared" si="2"/>
+        <v>- id: 3%name_en: 'Almond chicken '%name_ch: '杏仁雞 '%price: 7%spicy: %type: 'lunch'</v>
+      </c>
+      <c r="I60" t="str">
+        <f t="shared" si="3"/>
+        <v>- id: 3%name_en: "Almond chicken "%name_ch: "杏仁雞 "%price: 7%spicy: %type: "lunch"</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>4</v>
+      </c>
+      <c r="B61" t="s">
+        <v>257</v>
+      </c>
+      <c r="C61" t="s">
+        <v>258</v>
+      </c>
+      <c r="F61">
+        <v>7</v>
+      </c>
+      <c r="G61" t="s">
+        <v>252</v>
+      </c>
+      <c r="H61" t="str">
+        <f t="shared" si="2"/>
+        <v>- id: 4%name_en: 'Chicken with mixed vegetables '%name_ch: '時菜雞 '%price: 7%spicy: %type: 'lunch'</v>
+      </c>
+      <c r="I61" t="str">
+        <f t="shared" si="3"/>
+        <v>- id: 4%name_en: "Chicken with mixed vegetables "%name_ch: "時菜雞 "%price: 7%spicy: %type: "lunch"</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>5</v>
+      </c>
+      <c r="B62" t="s">
+        <v>259</v>
+      </c>
+      <c r="C62" t="s">
+        <v>260</v>
+      </c>
+      <c r="F62">
+        <v>7</v>
+      </c>
+      <c r="G62" t="s">
+        <v>252</v>
+      </c>
+      <c r="H62" t="str">
+        <f t="shared" si="2"/>
+        <v>- id: 5%name_en: 'Tofu with mixed vegetables '%name_ch: '時菜豆腐 '%price: 7%spicy: %type: 'lunch'</v>
+      </c>
+      <c r="I62" t="str">
+        <f t="shared" si="3"/>
+        <v>- id: 5%name_en: "Tofu with mixed vegetables "%name_ch: "時菜豆腐 "%price: 7%spicy: %type: "lunch"</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>6</v>
+      </c>
+      <c r="B63" t="s">
+        <v>261</v>
+      </c>
+      <c r="C63" t="s">
+        <v>262</v>
+      </c>
+      <c r="F63">
+        <v>7.5</v>
+      </c>
+      <c r="G63" t="s">
+        <v>252</v>
+      </c>
+      <c r="H63" t="str">
+        <f t="shared" si="2"/>
+        <v>- id: 6%name_en: 'Mongolian beef '%name_ch: '蒙古牛肉 '%price: 7.5%spicy: %type: 'lunch'</v>
+      </c>
+      <c r="I63" t="str">
+        <f t="shared" si="3"/>
+        <v>- id: 6%name_en: "Mongolian beef "%name_ch: "蒙古牛肉 "%price: 7.5%spicy: %type: "lunch"</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>7</v>
+      </c>
+      <c r="B64" t="s">
+        <v>263</v>
+      </c>
+      <c r="C64" t="s">
+        <v>147</v>
+      </c>
+      <c r="F64">
+        <v>7</v>
+      </c>
+      <c r="G64" t="s">
+        <v>252</v>
+      </c>
+      <c r="H64" t="str">
+        <f t="shared" si="2"/>
+        <v>- id: 7%name_en: 'Beef with broccoli'%name_ch: '西蘭花牛肉 '%price: 7%spicy: %type: 'lunch'</v>
+      </c>
+      <c r="I64" t="str">
+        <f t="shared" si="3"/>
+        <v>- id: 7%name_en: "Beef with broccoli"%name_ch: "西蘭花牛肉 "%price: 7%spicy: %type: "lunch"</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>8</v>
+      </c>
+      <c r="B65" t="s">
+        <v>264</v>
+      </c>
+      <c r="C65" t="s">
+        <v>265</v>
+      </c>
+      <c r="F65">
+        <v>7</v>
+      </c>
+      <c r="G65" t="s">
+        <v>252</v>
+      </c>
+      <c r="H65" t="str">
+        <f t="shared" si="2"/>
+        <v>- id: 8%name_en: 'Sweet &amp; sour pork '%name_ch: '甜酸肉'%price: 7%spicy: %type: 'lunch'</v>
+      </c>
+      <c r="I65" t="str">
+        <f t="shared" si="3"/>
+        <v>- id: 8%name_en: "Sweet &amp; sour pork "%name_ch: "甜酸肉"%price: 7%spicy: %type: "lunch"</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>9</v>
+      </c>
+      <c r="B66" t="s">
+        <v>266</v>
+      </c>
+      <c r="C66" t="s">
+        <v>267</v>
+      </c>
+      <c r="E66">
+        <v>2</v>
+      </c>
+      <c r="F66">
+        <v>7.5</v>
+      </c>
+      <c r="G66" t="s">
+        <v>252</v>
+      </c>
+      <c r="H66" t="str">
+        <f t="shared" si="2"/>
+        <v>- id: 9%name_en: 'Kung Pao prawns '%name_ch: '宮保蝦球 '%price: 7.5%spicy: 2%type: 'lunch'</v>
+      </c>
+      <c r="I66" t="str">
+        <f t="shared" si="3"/>
+        <v>- id: 9%name_en: "Kung Pao prawns "%name_ch: "宮保蝦球 "%price: 7.5%spicy: 2%type: "lunch"</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>10</v>
+      </c>
+      <c r="B67" t="s">
+        <v>268</v>
+      </c>
+      <c r="C67" t="s">
+        <v>269</v>
+      </c>
+      <c r="F67">
+        <v>7.5</v>
+      </c>
+      <c r="G67" t="s">
+        <v>252</v>
+      </c>
+      <c r="H67" t="str">
+        <f t="shared" si="2"/>
+        <v>- id: 10%name_en: 'Prawns with mixed vegetables '%name_ch: '時菜蝦球 '%price: 7.5%spicy: %type: 'lunch'</v>
+      </c>
+      <c r="I67" t="str">
+        <f t="shared" si="3"/>
+        <v>- id: 10%name_en: "Prawns with mixed vegetables "%name_ch: "時菜蝦球 "%price: 7.5%spicy: %type: "lunch"</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>11</v>
+      </c>
+      <c r="B68" t="s">
+        <v>270</v>
+      </c>
+      <c r="C68" t="s">
+        <v>271</v>
+      </c>
+      <c r="F68">
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="G68" t="s">
+        <v>252</v>
+      </c>
+      <c r="H68" t="str">
+        <f t="shared" si="2"/>
+        <v>- id: 11%name_en: 'Dry beef chow fon '%name_ch: '乾炒牛河 '%price: 8.95%spicy: %type: 'lunch'</v>
+      </c>
+      <c r="I68" t="str">
+        <f t="shared" si="3"/>
+        <v>- id: 11%name_en: "Dry beef chow fon "%name_ch: "乾炒牛河 "%price: 8.95%spicy: %type: "lunch"</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>12</v>
+      </c>
+      <c r="B69" t="s">
+        <v>29</v>
+      </c>
+      <c r="C69" t="s">
+        <v>28</v>
+      </c>
+      <c r="F69">
+        <v>7.5</v>
+      </c>
+      <c r="G69" t="s">
+        <v>252</v>
+      </c>
+      <c r="H69" t="str">
+        <f t="shared" si="2"/>
+        <v>- id: 12%name_en: 'Homemade pan fried noodles Shanghai style'%name_ch: '上海炒粗麵'%price: 7.5%spicy: %type: 'lunch'</v>
+      </c>
+      <c r="I69" t="str">
+        <f t="shared" si="3"/>
+        <v>- id: 12%name_en: "Homemade pan fried noodles Shanghai style"%name_ch: "上海炒粗麵"%price: 7.5%spicy: %type: "lunch"</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>